<commit_message>
archivos merma_y_diferencia para cada experimento (de antes)
</commit_message>
<xml_diff>
--- a/gama_codigo/models/resultados/finales/exp1-finales/merma_y_diferencia2.xlsx
+++ b/gama_codigo/models/resultados/finales/exp1-finales/merma_y_diferencia2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shali\OneDrive\Escritorio\GAMA_1.8.1\tesis\gama_codigo\models\resultados\finales\exp1-finales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2EC632-CF17-44EE-9D85-3644EDC13EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A25FAD-B7FD-4141-ACA9-5628A798F7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Producto</t>
   </si>
@@ -116,12 +116,24 @@
   </si>
   <si>
     <t>merma (%)</t>
+  </si>
+  <si>
+    <t>diferencia2</t>
+  </si>
+  <si>
+    <t>diferencia3</t>
+  </si>
+  <si>
+    <t>diferencia4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,9 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,22 +447,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,14 +477,26 @@
       <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -482,7 +509,7 @@
       <c r="D2">
         <v>2220500</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f>SUM(B2,C2*-1)/B2*100</f>
         <v>88.535458928588383</v>
       </c>
@@ -490,8 +517,23 @@
         <f>(B2/D2)</f>
         <v>55.491191173159201</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>SUM(D2,-B2)/D2</f>
+        <v>-54.491191173159201</v>
+      </c>
+      <c r="H2">
+        <f>SUM((B2/D2)*100,-100)</f>
+        <v>5449.1191173159204</v>
+      </c>
+      <c r="I2">
+        <f>SUM((B2/D2),-1)</f>
+        <v>54.491191173159201</v>
+      </c>
+      <c r="K2" s="2">
+        <v>54.491191173159201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -504,7 +546,7 @@
       <c r="D3">
         <v>365700</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E22" si="0">SUM(B3,C3*-1)/B3*100</f>
         <v>0</v>
       </c>
@@ -512,8 +554,23 @@
         <f t="shared" ref="F3:F22" si="1">(B3/D3)</f>
         <v>29.989433962264151</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" ref="G3:G22" si="2">SUM(D3,-B3)/D3</f>
+        <v>-28.989433962264151</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H22" si="3">SUM((B3/D3)*100,-100)</f>
+        <v>2898.9433962264152</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:K22" si="4">SUM((B3/D3),-1)</f>
+        <v>28.989433962264151</v>
+      </c>
+      <c r="K3" s="2">
+        <v>28.989433962264151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -526,7 +583,7 @@
       <c r="D4">
         <v>450000</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>97.578089606939088</v>
       </c>
@@ -534,8 +591,23 @@
         <f t="shared" si="1"/>
         <v>1769.4931200000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>-1768.4931200000001</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>176849.31200000001</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>1768.4931200000001</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1768.4931200000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -548,7 +620,7 @@
       <c r="D5">
         <v>116750</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>87.521058703575576</v>
       </c>
@@ -556,8 +628,23 @@
         <f t="shared" si="1"/>
         <v>1417.2475546038545</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>-1416.2475546038545</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>141624.75546038544</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>1416.2475546038545</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1416.2475546038545</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -568,18 +655,33 @@
         <v>47355840</v>
       </c>
       <c r="D6">
-        <v>4899440</v>
-      </c>
-      <c r="E6">
+        <v>5033240</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>83.602094865428938</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>58.943881545646036</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57.376960168797829</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>-56.376960168797829</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>5637.6960168797832</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>56.376960168797829</v>
+      </c>
+      <c r="K6" s="2">
+        <v>56.376960168797829</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -592,7 +694,7 @@
       <c r="D7">
         <v>479372400</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -600,8 +702,23 @@
         <f t="shared" si="1"/>
         <v>2.5338039903840939E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f>SUM(D7,-B7)/D7</f>
+        <v>0.97466196009615902</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>-97.466196009615899</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>-0.97466196009615902</v>
+      </c>
+      <c r="K7" s="2">
+        <v>-0.97466196009615902</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -611,19 +728,34 @@
       <c r="C8">
         <v>23879424</v>
       </c>
-      <c r="D8" s="1">
-        <v>17291000</v>
-      </c>
-      <c r="E8">
+      <c r="D8">
+        <v>18756600</v>
+      </c>
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>1.3810319819559309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.2731211413582419</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>-0.27312114135824189</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>27.312114135824189</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>0.27312114135824195</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.27312114135824195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -634,18 +766,33 @@
         <v>40020820</v>
       </c>
       <c r="D9">
-        <v>4880610</v>
-      </c>
-      <c r="E9">
+        <v>5013010</v>
+      </c>
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>93.357304651025871</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>123.4433054474748</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>120.1830100079593</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>-119.1830100079593</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>11918.301000795929</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>119.1830100079593</v>
+      </c>
+      <c r="K9" s="2">
+        <v>119.1830100079593</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -658,7 +805,7 @@
       <c r="D10" s="1">
         <v>1166600</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
         <v>94.136861339002493</v>
       </c>
@@ -666,8 +813,23 @@
         <f t="shared" si="1"/>
         <v>394.26161066346646</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>-393.26161066346646</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>39326.161066346649</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>393.26161066346646</v>
+      </c>
+      <c r="K10" s="2">
+        <v>393.26161066346646</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -680,7 +842,7 @@
       <c r="D11">
         <v>1639500</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -688,8 +850,23 @@
         <f t="shared" si="1"/>
         <v>6.1696017078377556</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>-5.1696017078377556</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>516.96017078377554</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>5.1696017078377556</v>
+      </c>
+      <c r="K11" s="2">
+        <v>5.1696017078377556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -702,7 +879,7 @@
       <c r="D12">
         <v>1009980</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>48.11479189232999</v>
       </c>
@@ -710,8 +887,23 @@
         <f t="shared" si="1"/>
         <v>73.085402681241206</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>-72.085402681241206</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>7208.5402681241203</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>72.085402681241206</v>
+      </c>
+      <c r="K12" s="2">
+        <v>72.085402681241206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -724,7 +916,7 @@
       <c r="D13" s="1">
         <v>385900</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>94.302125029975471</v>
       </c>
@@ -732,8 +924,23 @@
         <f t="shared" si="1"/>
         <v>103.39283752267427</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>-102.39283752267427</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>10239.283752267427</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>102.39283752267427</v>
+      </c>
+      <c r="K13" s="2">
+        <v>102.39283752267427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -744,18 +951,33 @@
         <v>21864640</v>
       </c>
       <c r="D14">
-        <v>698600</v>
-      </c>
-      <c r="E14">
+        <v>1078000</v>
+      </c>
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>20.180512925950207</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>39.210720011451471</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25.410583487940631</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>-24.410583487940631</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>2441.058348794063</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>24.410583487940631</v>
+      </c>
+      <c r="K14" s="2">
+        <v>24.410583487940631</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -766,18 +988,33 @@
         <v>27348254</v>
       </c>
       <c r="D15">
-        <v>1788500</v>
-      </c>
-      <c r="E15">
+        <v>1789750</v>
+      </c>
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>15.291168017892089</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15.280488336359827</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>-14.280488336359827</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>1428.0488336359826</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>14.280488336359827</v>
+      </c>
+      <c r="K15" s="2">
+        <v>14.280488336359827</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -790,7 +1027,7 @@
       <c r="D16">
         <v>145250</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <f t="shared" si="0"/>
         <v>95.622220156618837</v>
       </c>
@@ -798,8 +1035,23 @@
         <f t="shared" si="1"/>
         <v>1774.717982788296</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>-1773.717982788296</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>177371.79827882961</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>1773.717982788296</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1773.717982788296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -812,7 +1064,7 @@
       <c r="D17">
         <v>10900</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <f t="shared" si="0"/>
         <v>91.142378739814404</v>
       </c>
@@ -820,8 +1072,23 @@
         <f t="shared" si="1"/>
         <v>36694.110366972476</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>-36693.110366972476</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>3669311.0366972475</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>36693.110366972476</v>
+      </c>
+      <c r="K17" s="2">
+        <v>36693.110366972476</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -834,7 +1101,7 @@
       <c r="D18">
         <v>4598640</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -842,8 +1109,23 @@
         <f t="shared" si="1"/>
         <v>4.8445418645512586</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>-3.8445418645512586</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>384.45418645512586</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>3.8445418645512586</v>
+      </c>
+      <c r="K18" s="2">
+        <v>3.8445418645512586</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -856,7 +1138,7 @@
       <c r="D19">
         <v>2927400</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>22.29332687385131</v>
       </c>
@@ -864,8 +1146,23 @@
         <f t="shared" si="1"/>
         <v>5.7593663318986135</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>-4.7593663318986135</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>475.93663318986137</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>4.7593663318986135</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4.7593663318986135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -876,18 +1173,33 @@
         <v>4646430</v>
       </c>
       <c r="D20">
-        <v>2492252</v>
-      </c>
-      <c r="E20">
+        <v>2533993</v>
+      </c>
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>1.8643499934998546</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.833639635152899</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>-0.83363963515289896</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>83.363963515289896</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>0.83363963515289896</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.83363963515289896</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -898,18 +1210,33 @@
         <v>4139008</v>
       </c>
       <c r="D21">
-        <v>278130</v>
-      </c>
-      <c r="E21">
+        <v>369330</v>
+      </c>
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>91.509286010696727</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>175.26864056376513</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>131.98891777001597</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>-130.98891777001597</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>13098.891777001598</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>130.98891777001597</v>
+      </c>
+      <c r="K21" s="2">
+        <v>130.98891777001597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -919,19 +1246,35 @@
       <c r="C22">
         <v>42951976</v>
       </c>
-      <c r="D22" s="1">
-        <v>3576960</v>
-      </c>
-      <c r="E22">
+      <c r="D22">
+        <v>3656760</v>
+      </c>
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>6.1481598696806428</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>12.794587023617821</v>
+        <v>12.515375906540216</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>-11.515375906540216</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>1151.5375906540216</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>11.515375906540216</v>
+      </c>
+      <c r="K22" s="2">
+        <v>11.515375906540216</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>